<commit_message>
add "import csv file" function  and edit save, load student functions
</commit_message>
<xml_diff>
--- a/CS162-Final Project/19CLC9 Students.xlsx
+++ b/CS162-Final Project/19CLC9 Students.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="19CLC9 Students" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -110,9 +110,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -448,14 +452,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -468,14 +472,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>37145</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -488,14 +492,14 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>37109</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,14 +512,14 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>37166</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,14 +532,14 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <v>37246</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,30 +552,15 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
         <v>37035</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>